<commit_message>
[UPDATE] GomSpace.xlsx change currency->accounting and add custom format for Quarter to be consistent for python interpretability
</commit_message>
<xml_diff>
--- a/financial_data/GomSpace.xlsx
+++ b/financial_data/GomSpace.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C553AB-AAF1-4B6F-BAE5-18D1DE06531F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1085D7-6BE4-4DA1-8D2C-F412372116B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D4168B6-43E9-4474-9A7A-6AA1A32D8675}"/>
   </bookViews>
@@ -201,8 +201,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$SEK]\ #,##0.00_);[Red]\([$SEK]\ #,##0.00\)"/>
+  <numFmts count="2">
+    <numFmt numFmtId="167" formatCode="_([$SEK]\ * #,##0.00_);_([$SEK]\ * \(#,##0.00\);_([$SEK]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -259,16 +260,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -611,44 +612,43 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" style="5" customWidth="1"/>
-    <col min="18" max="18" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="30" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="44" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="48" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="53" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="56" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="16384" width="9" style="5"/>
+    <col min="1" max="1" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="19" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" style="3" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="30" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="42" max="44" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="46" max="48" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="51" max="53" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="54" max="56" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="57" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56" s="2" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
@@ -822,2916 +822,2916 @@
       </c>
     </row>
     <row r="2" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="6">
         <v>43830</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="5">
         <v>136263</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="5">
         <v>-118269</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="5">
         <v>17994</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
         <v>-43789</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="5">
         <v>-40635</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="5">
         <v>-45030</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="5">
         <v>303</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="5">
         <v>-2699</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="5">
         <v>-113856</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="5">
         <v>-25967</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="5">
         <v>485</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="5">
         <v>-7193</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="5">
         <v>-146531</v>
       </c>
-      <c r="O2" s="4">
+      <c r="O2" s="5">
         <v>-5132</v>
       </c>
-      <c r="P2" s="4">
+      <c r="P2" s="5">
         <v>-151663</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="Q2" s="5">
         <v>3710</v>
       </c>
-      <c r="R2" s="4">
+      <c r="R2" s="5">
         <v>116844</v>
       </c>
-      <c r="S2" s="4">
+      <c r="S2" s="5">
         <v>31062</v>
       </c>
-      <c r="T2" s="4">
+      <c r="T2" s="5">
         <v>54541</v>
       </c>
-      <c r="U2" s="4">
+      <c r="U2" s="5">
         <v>11672</v>
       </c>
-      <c r="V2" s="4">
+      <c r="V2" s="5">
         <v>1173</v>
       </c>
-      <c r="W2" s="4">
+      <c r="W2" s="5">
         <v>4071</v>
       </c>
-      <c r="X2" s="4">
+      <c r="X2" s="5">
         <v>223073</v>
       </c>
-      <c r="Y2" s="4">
+      <c r="Y2" s="5">
         <v>24133</v>
       </c>
-      <c r="Z2" s="4">
+      <c r="Z2" s="5">
         <v>13087</v>
       </c>
-      <c r="AA2" s="4">
+      <c r="AA2" s="5">
         <v>37212</v>
       </c>
-      <c r="AB2" s="4">
+      <c r="AB2" s="5">
         <v>6588</v>
       </c>
-      <c r="AC2" s="4">
+      <c r="AC2" s="5">
         <v>4125</v>
       </c>
-      <c r="AD2" s="4">
+      <c r="AD2" s="5">
         <v>1375</v>
       </c>
-      <c r="AE2" s="4">
+      <c r="AE2" s="5">
         <v>127160</v>
       </c>
-      <c r="AF2" s="4">
+      <c r="AF2" s="5">
         <v>213680</v>
       </c>
-      <c r="AG2" s="4">
+      <c r="AG2" s="5">
         <v>436753</v>
       </c>
-      <c r="AH2" s="4">
+      <c r="AH2" s="5">
         <v>3660</v>
       </c>
-      <c r="AI2" s="4">
+      <c r="AI2" s="5">
         <v>581599</v>
       </c>
-      <c r="AJ2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="4">
+      <c r="AJ2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="5">
         <v>7771</v>
       </c>
-      <c r="AL2" s="4">
+      <c r="AL2" s="5">
         <v>-297348</v>
       </c>
-      <c r="AM2" s="4">
+      <c r="AM2" s="5">
         <v>295682</v>
       </c>
-      <c r="AN2" s="4">
+      <c r="AN2" s="5">
         <v>14874</v>
       </c>
-      <c r="AO2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP2" s="4">
+      <c r="AO2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="5">
         <v>43956</v>
       </c>
-      <c r="AQ2" s="4">
+      <c r="AQ2" s="5">
         <v>2933</v>
       </c>
-      <c r="AR2" s="4">
+      <c r="AR2" s="5">
         <v>61763</v>
       </c>
-      <c r="AS2" s="4">
+      <c r="AS2" s="5">
         <v>8966</v>
       </c>
-      <c r="AT2" s="4">
+      <c r="AT2" s="5">
         <v>10769</v>
       </c>
-      <c r="AU2" s="4">
+      <c r="AU2" s="5">
         <v>9621</v>
       </c>
-      <c r="AV2" s="4">
+      <c r="AV2" s="5">
         <v>29156</v>
       </c>
-      <c r="AW2" s="4">
+      <c r="AW2" s="5">
         <v>4132</v>
       </c>
-      <c r="AX2" s="4">
+      <c r="AX2" s="5">
         <v>163</v>
       </c>
-      <c r="AY2" s="4">
-        <v>0</v>
-      </c>
-      <c r="AZ2" s="4">
+      <c r="AY2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="5">
         <v>16501</v>
       </c>
-      <c r="BA2" s="4">
-        <v>0</v>
-      </c>
-      <c r="BB2" s="4">
+      <c r="BA2" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB2" s="5">
         <v>79308</v>
       </c>
-      <c r="BC2" s="4">
+      <c r="BC2" s="5">
         <v>141071</v>
       </c>
-      <c r="BD2" s="4">
+      <c r="BD2" s="5">
         <v>436753</v>
       </c>
     </row>
     <row r="3" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="6">
         <v>43921</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="5">
         <v>150761.58743169397</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="5">
         <v>-125395.09562841531</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="5">
         <v>25366.491803278688</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="5">
         <v>-40022.445355191259</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="5">
         <v>-35600.661202185787</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="5">
         <v>-41510.587431693988</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="5">
         <v>723.68852459016398</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="5">
         <v>-2027.9371584699454</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="5">
         <v>-93071.450819672129</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="5">
         <v>-21755.639344262294</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="5">
         <v>804.74316939890707</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="5">
         <v>-7925.7240437158471</v>
       </c>
-      <c r="N3" s="4">
+      <c r="N3" s="5">
         <v>-121948.07103825136</v>
       </c>
-      <c r="O3" s="4">
+      <c r="O3" s="5">
         <v>-2838.3524590163934</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P3" s="5">
         <v>-124786.42349726777</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="Q3" s="5">
         <v>3710</v>
       </c>
-      <c r="R3" s="4">
+      <c r="R3" s="5">
         <v>116110.28142076504</v>
       </c>
-      <c r="S3" s="4">
+      <c r="S3" s="5">
         <v>28905.349726775956</v>
       </c>
-      <c r="T3" s="4">
+      <c r="T3" s="5">
         <v>51585.986338797818</v>
       </c>
-      <c r="U3" s="4">
+      <c r="U3" s="5">
         <v>8769.9453551912557</v>
       </c>
-      <c r="V3" s="4">
+      <c r="V3" s="5">
         <v>1264.4972677595629</v>
       </c>
-      <c r="W3" s="4">
+      <c r="W3" s="5">
         <v>4070.5027322404371</v>
       </c>
-      <c r="X3" s="4">
+      <c r="X3" s="5">
         <v>214416.56284153007</v>
       </c>
-      <c r="Y3" s="4">
+      <c r="Y3" s="5">
         <v>24708.836065573771</v>
       </c>
-      <c r="Z3" s="4">
+      <c r="Z3" s="5">
         <v>14717.043715846994</v>
       </c>
-      <c r="AA3" s="4">
+      <c r="AA3" s="5">
         <v>33362.401639344258</v>
       </c>
-      <c r="AB3" s="4">
+      <c r="AB3" s="5">
         <v>6206.0983606557384</v>
       </c>
-      <c r="AC3" s="4">
+      <c r="AC3" s="5">
         <v>3683.1775956284155</v>
       </c>
-      <c r="AD3" s="4">
+      <c r="AD3" s="5">
         <v>2044.5710382513662</v>
       </c>
-      <c r="AE3" s="4">
+      <c r="AE3" s="5">
         <v>129234.10382513661</v>
       </c>
-      <c r="AF3" s="4">
+      <c r="AF3" s="5">
         <v>213956.23224043715</v>
       </c>
-      <c r="AG3" s="4">
+      <c r="AG3" s="5">
         <v>428372.79508196726</v>
       </c>
-      <c r="AH3" s="4">
+      <c r="AH3" s="5">
         <v>3660</v>
       </c>
-      <c r="AI3" s="4">
+      <c r="AI3" s="5">
         <v>581599</v>
       </c>
-      <c r="AJ3" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="4">
+      <c r="AJ3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="5">
         <v>6481.0874316939889</v>
       </c>
-      <c r="AL3" s="4">
+      <c r="AL3" s="5">
         <v>-308057.40710382513</v>
       </c>
-      <c r="AM3" s="4">
+      <c r="AM3" s="5">
         <v>283682.68032786885</v>
       </c>
-      <c r="AN3" s="4">
+      <c r="AN3" s="5">
         <v>14722.333333333332</v>
       </c>
-      <c r="AO3" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="4">
+      <c r="AO3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="5">
         <v>40919.93169398907</v>
       </c>
-      <c r="AQ3" s="4">
+      <c r="AQ3" s="5">
         <v>4131.166666666667</v>
       </c>
-      <c r="AR3" s="4">
+      <c r="AR3" s="5">
         <v>59773.43169398907</v>
       </c>
-      <c r="AS3" s="4">
+      <c r="AS3" s="5">
         <v>7883.6967213114749</v>
       </c>
-      <c r="AT3" s="4">
+      <c r="AT3" s="5">
         <v>10801.571038251366</v>
       </c>
-      <c r="AU3" s="4">
+      <c r="AU3" s="5">
         <v>12743.592896174863</v>
       </c>
-      <c r="AV3" s="4">
+      <c r="AV3" s="5">
         <v>32902.166666666672</v>
       </c>
-      <c r="AW3" s="4">
+      <c r="AW3" s="5">
         <v>3557.1584699453551</v>
       </c>
-      <c r="AX3" s="4">
+      <c r="AX3" s="5">
         <v>417.60109289617486</v>
       </c>
-      <c r="AY3" s="4">
-        <v>0</v>
-      </c>
-      <c r="AZ3" s="4">
+      <c r="AY3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ3" s="5">
         <v>16610.896174863388</v>
       </c>
-      <c r="BA3" s="4">
-        <v>0</v>
-      </c>
-      <c r="BB3" s="4">
+      <c r="BA3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB3" s="5">
         <v>84916.683060109295</v>
       </c>
-      <c r="BC3" s="4">
+      <c r="BC3" s="5">
         <v>144690.11475409835</v>
       </c>
-      <c r="BD3" s="4">
+      <c r="BD3" s="5">
         <v>428372.79508196726</v>
       </c>
     </row>
     <row r="4" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="6">
         <v>44012</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="5">
         <v>165260.17486338798</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="5">
         <v>-132521.19125683061</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="5">
         <v>32738.983606557376</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="5">
         <v>-36255.890710382511</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="5">
         <v>-30566.322404371582</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="5">
         <v>-37991.174863387976</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="5">
         <v>1144.377049180328</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="5">
         <v>-1356.8743169398908</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="5">
         <v>-72286.901639344258</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="5">
         <v>-17544.278688524591</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="5">
         <v>1124.4863387978141</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="5">
         <v>-8658.4480874316941</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="5">
         <v>-97365.142076502729</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="5">
         <v>-544.70491803278674</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="5">
         <v>-97909.846994535517</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q4" s="5">
         <v>3710</v>
       </c>
-      <c r="R4" s="4">
+      <c r="R4" s="5">
         <v>115376.56284153006</v>
       </c>
-      <c r="S4" s="4">
+      <c r="S4" s="5">
         <v>26748.699453551912</v>
       </c>
-      <c r="T4" s="4">
+      <c r="T4" s="5">
         <v>48630.97267759563</v>
       </c>
-      <c r="U4" s="4">
+      <c r="U4" s="5">
         <v>5867.8907103825131</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V4" s="5">
         <v>1355.9945355191257</v>
       </c>
-      <c r="W4" s="4">
+      <c r="W4" s="5">
         <v>4070.0054644808743</v>
       </c>
-      <c r="X4" s="4">
+      <c r="X4" s="5">
         <v>205760.12568306012</v>
       </c>
-      <c r="Y4" s="4">
+      <c r="Y4" s="5">
         <v>25284.672131147541</v>
       </c>
-      <c r="Z4" s="4">
+      <c r="Z4" s="5">
         <v>16347.087431693988</v>
       </c>
-      <c r="AA4" s="4">
+      <c r="AA4" s="5">
         <v>29512.803278688523</v>
       </c>
-      <c r="AB4" s="4">
+      <c r="AB4" s="5">
         <v>5824.1967213114758</v>
       </c>
-      <c r="AC4" s="4">
+      <c r="AC4" s="5">
         <v>3241.3551912568305</v>
       </c>
-      <c r="AD4" s="4">
+      <c r="AD4" s="5">
         <v>2714.1420765027324</v>
       </c>
-      <c r="AE4" s="4">
+      <c r="AE4" s="5">
         <v>131308.20765027322</v>
       </c>
-      <c r="AF4" s="4">
+      <c r="AF4" s="5">
         <v>214232.4644808743</v>
       </c>
-      <c r="AG4" s="4">
+      <c r="AG4" s="5">
         <v>419992.59016393445</v>
       </c>
-      <c r="AH4" s="4">
+      <c r="AH4" s="5">
         <v>3660</v>
       </c>
-      <c r="AI4" s="4">
+      <c r="AI4" s="5">
         <v>581599</v>
       </c>
-      <c r="AJ4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="4">
+      <c r="AJ4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="5">
         <v>5191.1748633879779</v>
       </c>
-      <c r="AL4" s="4">
+      <c r="AL4" s="5">
         <v>-318766.81420765026</v>
       </c>
-      <c r="AM4" s="4">
+      <c r="AM4" s="5">
         <v>271683.36065573769</v>
       </c>
-      <c r="AN4" s="4">
+      <c r="AN4" s="5">
         <v>14570.666666666666</v>
       </c>
-      <c r="AO4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP4" s="4">
+      <c r="AO4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="5">
         <v>37883.863387978141</v>
       </c>
-      <c r="AQ4" s="4">
+      <c r="AQ4" s="5">
         <v>5329.3333333333339</v>
       </c>
-      <c r="AR4" s="4">
+      <c r="AR4" s="5">
         <v>57783.863387978141</v>
       </c>
-      <c r="AS4" s="4">
+      <c r="AS4" s="5">
         <v>6801.3934426229507</v>
       </c>
-      <c r="AT4" s="4">
+      <c r="AT4" s="5">
         <v>10834.142076502732</v>
       </c>
-      <c r="AU4" s="4">
+      <c r="AU4" s="5">
         <v>15866.185792349726</v>
       </c>
-      <c r="AV4" s="4">
+      <c r="AV4" s="5">
         <v>36648.333333333336</v>
       </c>
-      <c r="AW4" s="4">
+      <c r="AW4" s="5">
         <v>2982.3169398907103</v>
       </c>
-      <c r="AX4" s="4">
+      <c r="AX4" s="5">
         <v>672.20218579234972</v>
       </c>
-      <c r="AY4" s="4">
-        <v>0</v>
-      </c>
-      <c r="AZ4" s="4">
+      <c r="AY4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="5">
         <v>16720.792349726777</v>
       </c>
-      <c r="BA4" s="4">
-        <v>0</v>
-      </c>
-      <c r="BB4" s="4">
+      <c r="BA4" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB4" s="5">
         <v>90525.366120218576</v>
       </c>
-      <c r="BC4" s="4">
+      <c r="BC4" s="5">
         <v>148309.22950819673</v>
       </c>
-      <c r="BD4" s="4">
+      <c r="BD4" s="5">
         <v>419992.59016393445</v>
       </c>
     </row>
     <row r="5" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="6">
         <v>44104</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="5">
         <v>179918.08743169397</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="5">
         <v>-139725.59562841529</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="5">
         <v>40192.491803278688</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="5">
         <v>-32447.945355191256</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <v>-25476.661202185791</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="5">
         <v>-34433.087431693988</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="5">
         <v>1569.688524590164</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="5">
         <v>-678.43715846994542</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="5">
         <v>-51273.950819672129</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="5">
         <v>-13286.639344262296</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="5">
         <v>1447.743169398907</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="5">
         <v>-9399.2240437158471</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="5">
         <v>-72512.071038251364</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5" s="5">
         <v>1774.1475409836066</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="5">
         <v>-70737.923497267766</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5" s="5">
         <v>3710</v>
       </c>
-      <c r="R5" s="4">
+      <c r="R5" s="5">
         <v>114634.78142076504</v>
       </c>
-      <c r="S5" s="4">
+      <c r="S5" s="5">
         <v>24568.349726775956</v>
       </c>
-      <c r="T5" s="4">
+      <c r="T5" s="5">
         <v>45643.486338797811</v>
       </c>
-      <c r="U5" s="4">
+      <c r="U5" s="5">
         <v>2933.9453551912566</v>
       </c>
-      <c r="V5" s="4">
+      <c r="V5" s="5">
         <v>1448.4972677595629</v>
       </c>
-      <c r="W5" s="4">
+      <c r="W5" s="5">
         <v>4069.5027322404371</v>
       </c>
-      <c r="X5" s="4">
+      <c r="X5" s="5">
         <v>197008.56284153007</v>
       </c>
-      <c r="Y5" s="4">
+      <c r="Y5" s="5">
         <v>25866.836065573771</v>
       </c>
-      <c r="Z5" s="4">
+      <c r="Z5" s="5">
         <v>17995.043715846994</v>
       </c>
-      <c r="AA5" s="4">
+      <c r="AA5" s="5">
         <v>25620.901639344262</v>
       </c>
-      <c r="AB5" s="4">
+      <c r="AB5" s="5">
         <v>5438.0983606557384</v>
       </c>
-      <c r="AC5" s="4">
+      <c r="AC5" s="5">
         <v>2794.6775956284155</v>
       </c>
-      <c r="AD5" s="4">
+      <c r="AD5" s="5">
         <v>3391.0710382513662</v>
       </c>
-      <c r="AE5" s="4">
+      <c r="AE5" s="5">
         <v>133405.10382513661</v>
       </c>
-      <c r="AF5" s="4">
+      <c r="AF5" s="5">
         <v>214511.73224043715</v>
       </c>
-      <c r="AG5" s="4">
+      <c r="AG5" s="5">
         <v>411520.29508196726</v>
       </c>
-      <c r="AH5" s="4">
+      <c r="AH5" s="5">
         <v>3660</v>
       </c>
-      <c r="AI5" s="4">
+      <c r="AI5" s="5">
         <v>581599</v>
       </c>
-      <c r="AJ5" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="4">
+      <c r="AJ5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="5">
         <v>3887.0874316939889</v>
       </c>
-      <c r="AL5" s="4">
+      <c r="AL5" s="5">
         <v>-329593.90710382513</v>
       </c>
-      <c r="AM5" s="4">
+      <c r="AM5" s="5">
         <v>259552.18032786885</v>
       </c>
-      <c r="AN5" s="4">
+      <c r="AN5" s="5">
         <v>14417.333333333332</v>
       </c>
-      <c r="AO5" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP5" s="4">
+      <c r="AO5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="5">
         <v>34814.43169398907</v>
       </c>
-      <c r="AQ5" s="4">
+      <c r="AQ5" s="5">
         <v>6540.666666666667</v>
       </c>
-      <c r="AR5" s="4">
+      <c r="AR5" s="5">
         <v>55772.43169398907</v>
       </c>
-      <c r="AS5" s="4">
+      <c r="AS5" s="5">
         <v>5707.1967213114749</v>
       </c>
-      <c r="AT5" s="4">
+      <c r="AT5" s="5">
         <v>10867.071038251366</v>
       </c>
-      <c r="AU5" s="4">
+      <c r="AU5" s="5">
         <v>19023.092896174865</v>
       </c>
-      <c r="AV5" s="4">
+      <c r="AV5" s="5">
         <v>40435.666666666672</v>
       </c>
-      <c r="AW5" s="4">
+      <c r="AW5" s="5">
         <v>2401.1584699453551</v>
       </c>
-      <c r="AX5" s="4">
+      <c r="AX5" s="5">
         <v>929.6010928961748</v>
       </c>
-      <c r="AY5" s="4">
-        <v>0</v>
-      </c>
-      <c r="AZ5" s="4">
+      <c r="AY5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="5">
         <v>16831.896174863388</v>
       </c>
-      <c r="BA5" s="4">
-        <v>0</v>
-      </c>
-      <c r="BB5" s="4">
+      <c r="BA5" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="5">
         <v>96195.683060109295</v>
       </c>
-      <c r="BC5" s="4">
+      <c r="BC5" s="5">
         <v>151968.11475409838</v>
       </c>
-      <c r="BD5" s="4">
+      <c r="BD5" s="5">
         <v>411520.29508196726</v>
       </c>
     </row>
     <row r="6" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="6">
         <v>44196</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="5">
         <v>194576</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <v>-146930</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="5">
         <v>47646</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="5">
         <v>-28640</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="5">
         <v>-20387</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="5">
         <v>-30875</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="5">
         <v>1995</v>
       </c>
-      <c r="I6" s="4">
-        <v>0</v>
-      </c>
-      <c r="J6" s="4">
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
         <v>-30261</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="5">
         <v>-9029</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="5">
         <v>1771</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="5">
         <v>-10140</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="5">
         <v>-47659</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="5">
         <v>4093</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="5">
         <v>-43566</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6" s="5">
         <v>3710</v>
       </c>
-      <c r="R6" s="4">
+      <c r="R6" s="5">
         <v>113893</v>
       </c>
-      <c r="S6" s="4">
+      <c r="S6" s="5">
         <v>22388</v>
       </c>
-      <c r="T6" s="4">
+      <c r="T6" s="5">
         <v>42656</v>
       </c>
-      <c r="U6" s="4">
-        <v>0</v>
-      </c>
-      <c r="V6" s="4">
+      <c r="U6" s="5">
+        <v>0</v>
+      </c>
+      <c r="V6" s="5">
         <v>1541</v>
       </c>
-      <c r="W6" s="4">
+      <c r="W6" s="5">
         <v>4069</v>
       </c>
-      <c r="X6" s="4">
+      <c r="X6" s="5">
         <v>188257</v>
       </c>
-      <c r="Y6" s="4">
+      <c r="Y6" s="5">
         <v>26449</v>
       </c>
-      <c r="Z6" s="4">
+      <c r="Z6" s="5">
         <v>19643</v>
       </c>
-      <c r="AA6" s="4">
+      <c r="AA6" s="5">
         <v>21729</v>
       </c>
-      <c r="AB6" s="4">
+      <c r="AB6" s="5">
         <v>5052</v>
       </c>
-      <c r="AC6" s="4">
+      <c r="AC6" s="5">
         <v>2348</v>
       </c>
-      <c r="AD6" s="4">
+      <c r="AD6" s="5">
         <v>4068</v>
       </c>
-      <c r="AE6" s="4">
+      <c r="AE6" s="5">
         <v>135502</v>
       </c>
-      <c r="AF6" s="4">
+      <c r="AF6" s="5">
         <v>214791</v>
       </c>
-      <c r="AG6" s="4">
+      <c r="AG6" s="5">
         <v>403048</v>
       </c>
-      <c r="AH6" s="4">
+      <c r="AH6" s="5">
         <v>3660</v>
       </c>
-      <c r="AI6" s="4">
+      <c r="AI6" s="5">
         <v>581599</v>
       </c>
-      <c r="AJ6" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="4">
+      <c r="AJ6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="5">
         <v>2583</v>
       </c>
-      <c r="AL6" s="4">
+      <c r="AL6" s="5">
         <v>-340421</v>
       </c>
-      <c r="AM6" s="4">
+      <c r="AM6" s="5">
         <v>247421</v>
       </c>
-      <c r="AN6" s="4">
+      <c r="AN6" s="5">
         <v>14264</v>
       </c>
-      <c r="AO6" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP6" s="4">
+      <c r="AO6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="5">
         <v>31745</v>
       </c>
-      <c r="AQ6" s="4">
+      <c r="AQ6" s="5">
         <v>7752</v>
       </c>
-      <c r="AR6" s="4">
+      <c r="AR6" s="5">
         <v>53761</v>
       </c>
-      <c r="AS6" s="4">
+      <c r="AS6" s="5">
         <v>4613</v>
       </c>
-      <c r="AT6" s="4">
+      <c r="AT6" s="5">
         <v>10900</v>
       </c>
-      <c r="AU6" s="4">
+      <c r="AU6" s="5">
         <v>22180</v>
       </c>
-      <c r="AV6" s="4">
+      <c r="AV6" s="5">
         <v>44223</v>
       </c>
-      <c r="AW6" s="4">
+      <c r="AW6" s="5">
         <v>1820</v>
       </c>
-      <c r="AX6" s="4">
+      <c r="AX6" s="5">
         <v>1187</v>
       </c>
-      <c r="AY6" s="4">
-        <v>0</v>
-      </c>
-      <c r="AZ6" s="4">
+      <c r="AY6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ6" s="5">
         <v>16943</v>
       </c>
-      <c r="BA6" s="4">
-        <v>0</v>
-      </c>
-      <c r="BB6" s="4">
+      <c r="BA6" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="5">
         <v>101866</v>
       </c>
-      <c r="BC6" s="4">
+      <c r="BC6" s="5">
         <v>155627</v>
       </c>
-      <c r="BD6" s="4">
+      <c r="BD6" s="5">
         <v>403048</v>
       </c>
     </row>
     <row r="7" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="6">
         <v>44286</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="5">
         <v>199268.08219178082</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <v>-151284.27397260274</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="5">
         <v>47983.808219178085</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="5">
         <v>-27720.767123287671</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="5">
         <v>-20810.863013698632</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="5">
         <v>-31081.136986301368</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="5">
         <v>1549.6849315068494</v>
       </c>
-      <c r="I7" s="4">
-        <v>0</v>
-      </c>
-      <c r="J7" s="4">
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
         <v>-30079.273972602739</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="5">
         <v>-6802.6712328767126</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="5">
         <v>1743.8767123287671</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="5">
         <v>-8460.3287671232883</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="5">
         <v>-43598.397260273974</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="5">
         <v>4036.5342465753424</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="5">
         <v>-39561.863013698632</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7" s="5">
         <v>3710</v>
       </c>
-      <c r="R7" s="4">
+      <c r="R7" s="5">
         <v>117290.80821917808</v>
       </c>
-      <c r="S7" s="4">
+      <c r="S7" s="5">
         <v>20873.287671232876</v>
       </c>
-      <c r="T7" s="4">
+      <c r="T7" s="5">
         <v>40324.630136986299</v>
       </c>
-      <c r="U7" s="4">
-        <v>0</v>
-      </c>
-      <c r="V7" s="4">
+      <c r="U7" s="5">
+        <v>0</v>
+      </c>
+      <c r="V7" s="5">
         <v>1248.8082191780823</v>
       </c>
-      <c r="W7" s="4">
+      <c r="W7" s="5">
         <v>4090.4520547945203</v>
       </c>
-      <c r="X7" s="4">
+      <c r="X7" s="5">
         <v>187537.98630136985</v>
       </c>
-      <c r="Y7" s="4">
+      <c r="Y7" s="5">
         <v>28794.424657534248</v>
       </c>
-      <c r="Z7" s="4">
+      <c r="Z7" s="5">
         <v>23395.136986301372</v>
       </c>
-      <c r="AA7" s="4">
+      <c r="AA7" s="5">
         <v>23263.438356164384</v>
       </c>
-      <c r="AB7" s="4">
+      <c r="AB7" s="5">
         <v>5233.4794520547948</v>
       </c>
-      <c r="AC7" s="4">
+      <c r="AC7" s="5">
         <v>2798</v>
       </c>
-      <c r="AD7" s="4">
+      <c r="AD7" s="5">
         <v>3670.027397260274</v>
       </c>
-      <c r="AE7" s="4">
+      <c r="AE7" s="5">
         <v>126568.32876712328</v>
       </c>
-      <c r="AF7" s="4">
+      <c r="AF7" s="5">
         <v>213722.83561643836</v>
       </c>
-      <c r="AG7" s="4">
+      <c r="AG7" s="5">
         <v>401260.82191780821</v>
       </c>
-      <c r="AH7" s="4">
+      <c r="AH7" s="5">
         <v>3660</v>
       </c>
-      <c r="AI7" s="4">
+      <c r="AI7" s="5">
         <v>581599</v>
       </c>
-      <c r="AJ7" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK7" s="4">
+      <c r="AJ7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="5">
         <v>3743.3835616438355</v>
       </c>
-      <c r="AL7" s="4">
+      <c r="AL7" s="5">
         <v>-347136.9726027397</v>
       </c>
-      <c r="AM7" s="4">
+      <c r="AM7" s="5">
         <v>241865.4109589041</v>
       </c>
-      <c r="AN7" s="4">
+      <c r="AN7" s="5">
         <v>13286.821917808218</v>
       </c>
-      <c r="AO7" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP7" s="4">
+      <c r="AO7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="5">
         <v>29594.123287671235</v>
       </c>
-      <c r="AQ7" s="4">
+      <c r="AQ7" s="5">
         <v>8463.6164383561645</v>
       </c>
-      <c r="AR7" s="4">
+      <c r="AR7" s="5">
         <v>51344.561643835616</v>
       </c>
-      <c r="AS7" s="4">
+      <c r="AS7" s="5">
         <v>4345.7123287671229</v>
       </c>
-      <c r="AT7" s="4">
+      <c r="AT7" s="5">
         <v>10634.438356164383</v>
       </c>
-      <c r="AU7" s="4">
+      <c r="AU7" s="5">
         <v>24312.876712328769</v>
       </c>
-      <c r="AV7" s="4">
+      <c r="AV7" s="5">
         <v>48030.369863013701</v>
       </c>
-      <c r="AW7" s="4">
+      <c r="AW7" s="5">
         <v>1923.8082191780823</v>
       </c>
-      <c r="AX7" s="4">
+      <c r="AX7" s="5">
         <v>1256.7808219178082</v>
       </c>
-      <c r="AY7" s="4">
-        <v>0</v>
-      </c>
-      <c r="AZ7" s="4">
+      <c r="AY7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ7" s="5">
         <v>17410.013698630137</v>
       </c>
-      <c r="BA7" s="4">
+      <c r="BA7" s="5">
         <v>136.84931506849315</v>
       </c>
-      <c r="BB7" s="4">
+      <c r="BB7" s="5">
         <v>108050.8493150685</v>
       </c>
-      <c r="BC7" s="4">
+      <c r="BC7" s="5">
         <v>159395.4109589041</v>
       </c>
-      <c r="BD7" s="4">
+      <c r="BD7" s="5">
         <v>401260.82191780821</v>
       </c>
     </row>
     <row r="8" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="6">
         <v>44377</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="5">
         <v>204012.298630137</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="5">
         <v>-155686.92876712329</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="5">
         <v>48325.369863013701</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="5">
         <v>-26791.320547945204</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="5">
         <v>-21239.435616438357</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="5">
         <v>-31289.564383561643</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="5">
         <v>1099.4219178082192</v>
       </c>
-      <c r="I8" s="4">
-        <v>0</v>
-      </c>
-      <c r="J8" s="4">
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
         <v>-29895.528767123287</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="5">
         <v>-4551.6054794520551</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="5">
         <v>1716.4520547945206</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8" s="5">
         <v>-6761.9945205479453</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8" s="5">
         <v>-39492.676712328765</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O8" s="5">
         <v>3979.4410958904109</v>
       </c>
-      <c r="P8" s="4">
+      <c r="P8" s="5">
         <v>-35513.235616438353</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="Q8" s="5">
         <v>3710</v>
       </c>
-      <c r="R8" s="4">
+      <c r="R8" s="5">
         <v>120726.36986301369</v>
       </c>
-      <c r="S8" s="4">
+      <c r="S8" s="5">
         <v>19341.745205479452</v>
       </c>
-      <c r="T8" s="4">
+      <c r="T8" s="5">
         <v>37967.356164383564</v>
       </c>
-      <c r="U8" s="4">
-        <v>0</v>
-      </c>
-      <c r="V8" s="4">
+      <c r="U8" s="5">
+        <v>0</v>
+      </c>
+      <c r="V8" s="5">
         <v>953.3698630136987</v>
       </c>
-      <c r="W8" s="4">
+      <c r="W8" s="5">
         <v>4112.1424657534244</v>
       </c>
-      <c r="X8" s="4">
+      <c r="X8" s="5">
         <v>186810.98356164384</v>
       </c>
-      <c r="Y8" s="4">
+      <c r="Y8" s="5">
         <v>31165.909589041097</v>
       </c>
-      <c r="Z8" s="4">
+      <c r="Z8" s="5">
         <v>27188.964383561644</v>
       </c>
-      <c r="AA8" s="4">
+      <c r="AA8" s="5">
         <v>24814.926027397261</v>
       </c>
-      <c r="AB8" s="4">
+      <c r="AB8" s="5">
         <v>5416.9753424657538</v>
       </c>
-      <c r="AC8" s="4">
+      <c r="AC8" s="5">
         <v>3253</v>
       </c>
-      <c r="AD8" s="4">
+      <c r="AD8" s="5">
         <v>3267.6328767123287</v>
       </c>
-      <c r="AE8" s="4">
+      <c r="AE8" s="5">
         <v>117535.39452054794</v>
       </c>
-      <c r="AF8" s="4">
+      <c r="AF8" s="5">
         <v>212642.80273972603</v>
       </c>
-      <c r="AG8" s="4">
+      <c r="AG8" s="5">
         <v>399453.78630136984</v>
       </c>
-      <c r="AH8" s="4">
+      <c r="AH8" s="5">
         <v>3660</v>
       </c>
-      <c r="AI8" s="4">
+      <c r="AI8" s="5">
         <v>581599</v>
       </c>
-      <c r="AJ8" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK8" s="4">
+      <c r="AJ8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="5">
         <v>4916.6602739726022</v>
       </c>
-      <c r="AL8" s="4">
+      <c r="AL8" s="5">
         <v>-353927.56712328765</v>
       </c>
-      <c r="AM8" s="4">
+      <c r="AM8" s="5">
         <v>236248.09315068493</v>
       </c>
-      <c r="AN8" s="4">
+      <c r="AN8" s="5">
         <v>12298.786301369862</v>
       </c>
-      <c r="AO8" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP8" s="4">
+      <c r="AO8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="5">
         <v>27419.347945205482</v>
       </c>
-      <c r="AQ8" s="4">
+      <c r="AQ8" s="5">
         <v>9183.139726027397</v>
       </c>
-      <c r="AR8" s="4">
+      <c r="AR8" s="5">
         <v>48901.273972602743</v>
       </c>
-      <c r="AS8" s="4">
+      <c r="AS8" s="5">
         <v>4075.4547945205477</v>
       </c>
-      <c r="AT8" s="4">
+      <c r="AT8" s="5">
         <v>10365.92602739726</v>
       </c>
-      <c r="AU8" s="4">
+      <c r="AU8" s="5">
         <v>26469.452054794521</v>
       </c>
-      <c r="AV8" s="4">
+      <c r="AV8" s="5">
         <v>51880.043835616438</v>
       </c>
-      <c r="AW8" s="4">
+      <c r="AW8" s="5">
         <v>2028.7698630136986</v>
       </c>
-      <c r="AX8" s="4">
+      <c r="AX8" s="5">
         <v>1327.33698630137</v>
       </c>
-      <c r="AY8" s="4">
-        <v>0</v>
-      </c>
-      <c r="AZ8" s="4">
+      <c r="AY8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ8" s="5">
         <v>17882.216438356165</v>
       </c>
-      <c r="BA8" s="4">
+      <c r="BA8" s="5">
         <v>275.21917808219177</v>
       </c>
-      <c r="BB8" s="4">
+      <c r="BB8" s="5">
         <v>114304.41917808219</v>
       </c>
-      <c r="BC8" s="4">
+      <c r="BC8" s="5">
         <v>163205.69315068494</v>
       </c>
-      <c r="BD8" s="4">
+      <c r="BD8" s="5">
         <v>399453.78630136984</v>
       </c>
     </row>
     <row r="9" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="6">
         <v>44469</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="5">
         <v>208808.6493150685</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="5">
         <v>-160137.96438356163</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="5">
         <v>48670.684931506854</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="5">
         <v>-25851.6602739726</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="5">
         <v>-21672.717808219179</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="5">
         <v>-31500.282191780821</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="5">
         <v>644.21095890410959</v>
       </c>
-      <c r="I9" s="4">
-        <v>0</v>
-      </c>
-      <c r="J9" s="4">
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
         <v>-29709.764383561644</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="5">
         <v>-2275.8027397260275</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="5">
         <v>1688.7260273972602</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9" s="5">
         <v>-5044.9972602739726</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9" s="5">
         <v>-35341.838356164386</v>
       </c>
-      <c r="O9" s="4">
+      <c r="O9" s="5">
         <v>3921.7205479452055</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9" s="5">
         <v>-31420.117808219176</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="Q9" s="5">
         <v>3710</v>
       </c>
-      <c r="R9" s="4">
+      <c r="R9" s="5">
         <v>124199.68493150684</v>
       </c>
-      <c r="S9" s="4">
+      <c r="S9" s="5">
         <v>17793.372602739728</v>
       </c>
-      <c r="T9" s="4">
+      <c r="T9" s="5">
         <v>35584.178082191778</v>
       </c>
-      <c r="U9" s="4">
-        <v>0</v>
-      </c>
-      <c r="V9" s="4">
+      <c r="U9" s="5">
+        <v>0</v>
+      </c>
+      <c r="V9" s="5">
         <v>654.68493150684935</v>
       </c>
-      <c r="W9" s="4">
+      <c r="W9" s="5">
         <v>4134.0712328767122</v>
       </c>
-      <c r="X9" s="4">
+      <c r="X9" s="5">
         <v>186075.99178082193</v>
       </c>
-      <c r="Y9" s="4">
+      <c r="Y9" s="5">
         <v>33563.454794520549</v>
       </c>
-      <c r="Z9" s="4">
+      <c r="Z9" s="5">
         <v>31024.482191780822</v>
       </c>
-      <c r="AA9" s="4">
+      <c r="AA9" s="5">
         <v>26383.463013698631</v>
       </c>
-      <c r="AB9" s="4">
+      <c r="AB9" s="5">
         <v>5602.4876712328769</v>
       </c>
-      <c r="AC9" s="4">
+      <c r="AC9" s="5">
         <v>3713</v>
       </c>
-      <c r="AD9" s="4">
+      <c r="AD9" s="5">
         <v>2860.8164383561643</v>
       </c>
-      <c r="AE9" s="4">
+      <c r="AE9" s="5">
         <v>108403.19726027397</v>
       </c>
-      <c r="AF9" s="4">
+      <c r="AF9" s="5">
         <v>211550.90136986302</v>
       </c>
-      <c r="AG9" s="4">
+      <c r="AG9" s="5">
         <v>397626.89315068489</v>
       </c>
-      <c r="AH9" s="4">
+      <c r="AH9" s="5">
         <v>3660</v>
       </c>
-      <c r="AI9" s="4">
+      <c r="AI9" s="5">
         <v>581599</v>
       </c>
-      <c r="AJ9" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK9" s="4">
+      <c r="AJ9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="5">
         <v>6102.8301369863011</v>
       </c>
-      <c r="AL9" s="4">
+      <c r="AL9" s="5">
         <v>-360792.7835616438</v>
       </c>
-      <c r="AM9" s="4">
+      <c r="AM9" s="5">
         <v>230569.04657534248</v>
       </c>
-      <c r="AN9" s="4">
+      <c r="AN9" s="5">
         <v>11299.893150684931</v>
       </c>
-      <c r="AO9" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP9" s="4">
+      <c r="AO9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="5">
         <v>25220.673972602741</v>
       </c>
-      <c r="AQ9" s="4">
+      <c r="AQ9" s="5">
         <v>9910.5698630136976</v>
       </c>
-      <c r="AR9" s="4">
+      <c r="AR9" s="5">
         <v>46431.136986301368</v>
       </c>
-      <c r="AS9" s="4">
+      <c r="AS9" s="5">
         <v>3802.2273972602738</v>
       </c>
-      <c r="AT9" s="4">
+      <c r="AT9" s="5">
         <v>10094.463013698631</v>
       </c>
-      <c r="AU9" s="4">
+      <c r="AU9" s="5">
         <v>28649.726027397261</v>
       </c>
-      <c r="AV9" s="4">
+      <c r="AV9" s="5">
         <v>55772.021917808219</v>
       </c>
-      <c r="AW9" s="4">
+      <c r="AW9" s="5">
         <v>2134.8849315068492</v>
       </c>
-      <c r="AX9" s="4">
+      <c r="AX9" s="5">
         <v>1398.668493150685</v>
       </c>
-      <c r="AY9" s="4">
-        <v>0</v>
-      </c>
-      <c r="AZ9" s="4">
+      <c r="AY9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ9" s="5">
         <v>18359.608219178081</v>
       </c>
-      <c r="BA9" s="4">
+      <c r="BA9" s="5">
         <v>415.10958904109589</v>
       </c>
-      <c r="BB9" s="4">
+      <c r="BB9" s="5">
         <v>120626.7095890411</v>
       </c>
-      <c r="BC9" s="4">
+      <c r="BC9" s="5">
         <v>167057.84657534247</v>
       </c>
-      <c r="BD9" s="4">
+      <c r="BD9" s="5">
         <v>397626.89315068489</v>
       </c>
     </row>
     <row r="10" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="6">
         <v>44561</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="5">
         <v>213605</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="5">
         <v>-164589</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="5">
         <v>49016</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="5">
         <v>-24912</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="5">
         <v>-22106</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="5">
         <v>-31711</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="5">
         <v>189</v>
       </c>
-      <c r="I10" s="4">
-        <v>0</v>
-      </c>
-      <c r="J10" s="4">
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
         <v>-29524</v>
       </c>
-      <c r="K10" s="4">
-        <v>0</v>
-      </c>
-      <c r="L10" s="4">
+      <c r="K10" s="5">
+        <v>0</v>
+      </c>
+      <c r="L10" s="5">
         <v>1661</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="5">
         <v>-3328</v>
       </c>
-      <c r="N10" s="4">
+      <c r="N10" s="5">
         <v>-31191</v>
       </c>
-      <c r="O10" s="4">
+      <c r="O10" s="5">
         <v>3864</v>
       </c>
-      <c r="P10" s="4">
+      <c r="P10" s="5">
         <v>-27327</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="Q10" s="5">
         <v>3710</v>
       </c>
-      <c r="R10" s="4">
+      <c r="R10" s="5">
         <v>127673</v>
       </c>
-      <c r="S10" s="4">
+      <c r="S10" s="5">
         <v>16245</v>
       </c>
-      <c r="T10" s="4">
+      <c r="T10" s="5">
         <v>33201</v>
       </c>
-      <c r="U10" s="4">
-        <v>0</v>
-      </c>
-      <c r="V10" s="4">
+      <c r="U10" s="5">
+        <v>0</v>
+      </c>
+      <c r="V10" s="5">
         <v>356</v>
       </c>
-      <c r="W10" s="4">
+      <c r="W10" s="5">
         <v>4156</v>
       </c>
-      <c r="X10" s="4">
+      <c r="X10" s="5">
         <v>185341</v>
       </c>
-      <c r="Y10" s="4">
+      <c r="Y10" s="5">
         <v>35961</v>
       </c>
-      <c r="Z10" s="4">
+      <c r="Z10" s="5">
         <v>34860</v>
       </c>
-      <c r="AA10" s="4">
+      <c r="AA10" s="5">
         <v>27952</v>
       </c>
-      <c r="AB10" s="4">
+      <c r="AB10" s="5">
         <v>5788</v>
       </c>
-      <c r="AC10" s="4">
+      <c r="AC10" s="5">
         <v>4173</v>
       </c>
-      <c r="AD10" s="4">
+      <c r="AD10" s="5">
         <v>2454</v>
       </c>
-      <c r="AE10" s="4">
+      <c r="AE10" s="5">
         <v>99271</v>
       </c>
-      <c r="AF10" s="4">
+      <c r="AF10" s="5">
         <v>210459</v>
       </c>
-      <c r="AG10" s="4">
+      <c r="AG10" s="5">
         <v>395800</v>
       </c>
-      <c r="AH10" s="4">
+      <c r="AH10" s="5">
         <v>3660</v>
       </c>
-      <c r="AI10" s="4">
+      <c r="AI10" s="5">
         <v>581599</v>
       </c>
-      <c r="AJ10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK10" s="4">
+      <c r="AJ10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="5">
         <v>7289</v>
       </c>
-      <c r="AL10" s="4">
+      <c r="AL10" s="5">
         <v>-367658</v>
       </c>
-      <c r="AM10" s="4">
+      <c r="AM10" s="5">
         <v>224890</v>
       </c>
-      <c r="AN10" s="4">
+      <c r="AN10" s="5">
         <v>10301</v>
       </c>
-      <c r="AO10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP10" s="4">
+      <c r="AO10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="5">
         <v>23022</v>
       </c>
-      <c r="AQ10" s="4">
+      <c r="AQ10" s="5">
         <v>10638</v>
       </c>
-      <c r="AR10" s="4">
+      <c r="AR10" s="5">
         <v>43961</v>
       </c>
-      <c r="AS10" s="4">
+      <c r="AS10" s="5">
         <v>3529</v>
       </c>
-      <c r="AT10" s="4">
+      <c r="AT10" s="5">
         <v>9823</v>
       </c>
-      <c r="AU10" s="4">
+      <c r="AU10" s="5">
         <v>30830</v>
       </c>
-      <c r="AV10" s="4">
+      <c r="AV10" s="5">
         <v>59664</v>
       </c>
-      <c r="AW10" s="4">
+      <c r="AW10" s="5">
         <v>2241</v>
       </c>
-      <c r="AX10" s="4">
+      <c r="AX10" s="5">
         <v>1470</v>
       </c>
-      <c r="AY10" s="4">
-        <v>0</v>
-      </c>
-      <c r="AZ10" s="4">
+      <c r="AY10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ10" s="5">
         <v>18837</v>
       </c>
-      <c r="BA10" s="4">
+      <c r="BA10" s="5">
         <v>555</v>
       </c>
-      <c r="BB10" s="4">
+      <c r="BB10" s="5">
         <v>126949</v>
       </c>
-      <c r="BC10" s="4">
+      <c r="BC10" s="5">
         <v>170910</v>
       </c>
-      <c r="BD10" s="4">
+      <c r="BD10" s="5">
         <v>395800</v>
       </c>
     </row>
     <row r="11" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="6">
         <v>44651</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="5">
         <v>209850.64383561644</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="5">
         <v>-185525.46575342465</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="5">
         <v>24325.178082191782</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="5">
         <v>-34376.794520547948</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="5">
         <v>-34888.219178082189</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="5">
         <v>-34683.219178082189</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="5">
         <v>174.69863013698631</v>
       </c>
-      <c r="I11" s="4">
-        <v>0</v>
-      </c>
-      <c r="J11" s="4">
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
         <v>-79448.356164383556</v>
       </c>
-      <c r="K11" s="4">
-        <v>0</v>
-      </c>
-      <c r="L11" s="4">
+      <c r="K11" s="5">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5">
         <v>1719.9315068493152</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="5">
         <v>-3208.6575342465753</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11" s="5">
         <v>-80937.082191780821</v>
       </c>
-      <c r="O11" s="4">
+      <c r="O11" s="5">
         <v>4172.465753424658</v>
       </c>
-      <c r="P11" s="4">
+      <c r="P11" s="5">
         <v>-76764.61643835617</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="Q11" s="5">
         <v>2795.2054794520545</v>
       </c>
-      <c r="R11" s="4">
+      <c r="R11" s="5">
         <v>126356.04109589041</v>
       </c>
-      <c r="S11" s="4">
+      <c r="S11" s="5">
         <v>16866.863013698628</v>
       </c>
-      <c r="T11" s="4">
+      <c r="T11" s="5">
         <v>35760.452054794521</v>
       </c>
-      <c r="U11" s="4">
-        <v>0</v>
-      </c>
-      <c r="V11" s="4">
+      <c r="U11" s="5">
+        <v>0</v>
+      </c>
+      <c r="V11" s="5">
         <v>268.21917808219177</v>
       </c>
-      <c r="W11" s="4">
+      <c r="W11" s="5">
         <v>4313.3150684931506</v>
       </c>
-      <c r="X11" s="4">
+      <c r="X11" s="5">
         <v>186360.09589041094</v>
       </c>
-      <c r="Y11" s="4">
+      <c r="Y11" s="5">
         <v>38476.315068493153</v>
       </c>
-      <c r="Z11" s="4">
+      <c r="Z11" s="5">
         <v>33480.164383561641</v>
       </c>
-      <c r="AA11" s="4">
+      <c r="AA11" s="5">
         <v>25979.890410958906</v>
       </c>
-      <c r="AB11" s="4">
+      <c r="AB11" s="5">
         <v>6061.6986301369861</v>
       </c>
-      <c r="AC11" s="4">
+      <c r="AC11" s="5">
         <v>4138.4794520547948</v>
       </c>
-      <c r="AD11" s="4">
+      <c r="AD11" s="5">
         <v>3153.2876712328766</v>
       </c>
-      <c r="AE11" s="4">
+      <c r="AE11" s="5">
         <v>82954.123287671231</v>
       </c>
-      <c r="AF11" s="4">
+      <c r="AF11" s="5">
         <v>194243.9589041096</v>
       </c>
-      <c r="AG11" s="4">
+      <c r="AG11" s="5">
         <v>380604.05479452055</v>
       </c>
-      <c r="AH11" s="4">
+      <c r="AH11" s="5">
         <v>3840.2465753424658</v>
       </c>
-      <c r="AI11" s="4">
+      <c r="AI11" s="5">
         <v>605000.47945205483</v>
       </c>
-      <c r="AJ11" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK11" s="4">
+      <c r="AJ11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="5">
         <v>10053.356164383562</v>
       </c>
-      <c r="AL11" s="4">
+      <c r="AL11" s="5">
         <v>-423615.80821917811</v>
       </c>
-      <c r="AM11" s="4">
+      <c r="AM11" s="5">
         <v>195278.27397260274</v>
       </c>
-      <c r="AN11" s="4">
+      <c r="AN11" s="5">
         <v>9458.6986301369852</v>
       </c>
-      <c r="AO11" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP11" s="4">
+      <c r="AO11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="5">
         <v>25329.945205479453</v>
       </c>
-      <c r="AQ11" s="4">
+      <c r="AQ11" s="5">
         <v>10116</v>
       </c>
-      <c r="AR11" s="4">
+      <c r="AR11" s="5">
         <v>44904.643835616444</v>
       </c>
-      <c r="AS11" s="4">
+      <c r="AS11" s="5">
         <v>3701.3561643835615</v>
       </c>
-      <c r="AT11" s="4">
+      <c r="AT11" s="5">
         <v>10478.397260273972</v>
       </c>
-      <c r="AU11" s="4">
+      <c r="AU11" s="5">
         <v>30072.273972602739</v>
       </c>
-      <c r="AV11" s="4">
+      <c r="AV11" s="5">
         <v>57640.602739726033</v>
       </c>
-      <c r="AW11" s="4">
+      <c r="AW11" s="5">
         <v>2245.9315068493152</v>
       </c>
-      <c r="AX11" s="4">
+      <c r="AX11" s="5">
         <v>1383.6986301369864</v>
       </c>
-      <c r="AY11" s="4">
+      <c r="AY11" s="5">
         <v>13051.232876712329</v>
       </c>
-      <c r="AZ11" s="4">
+      <c r="AZ11" s="5">
         <v>18124.397260273974</v>
       </c>
-      <c r="BA11" s="4">
+      <c r="BA11" s="5">
         <v>3723.2465753424658</v>
       </c>
-      <c r="BB11" s="4">
+      <c r="BB11" s="5">
         <v>140421.13698630137</v>
       </c>
-      <c r="BC11" s="4">
+      <c r="BC11" s="5">
         <v>185325.78082191781</v>
       </c>
-      <c r="BD11" s="4">
+      <c r="BD11" s="5">
         <v>380604.05479452055</v>
       </c>
     </row>
     <row r="12" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="6">
         <v>44742</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="5">
         <v>206054.57260273973</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="5">
         <v>-206694.55890410958</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="5">
         <v>-639.98630136986321</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="5">
         <v>-43946.753424657538</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="5">
         <v>-47812.463013698623</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="5">
         <v>-37688.463013698631</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="5">
         <v>160.23835616438356</v>
       </c>
-      <c r="I12" s="4">
-        <v>0</v>
-      </c>
-      <c r="J12" s="4">
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
         <v>-129927.42739726027</v>
       </c>
-      <c r="K12" s="4">
-        <v>0</v>
-      </c>
-      <c r="L12" s="4">
+      <c r="K12" s="5">
+        <v>0</v>
+      </c>
+      <c r="L12" s="5">
         <v>1779.5178082191781</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="5">
         <v>-3087.9890410958906</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12" s="5">
         <v>-131235.89863013697</v>
       </c>
-      <c r="O12" s="4">
+      <c r="O12" s="5">
         <v>4484.3589041095893</v>
       </c>
-      <c r="P12" s="4">
+      <c r="P12" s="5">
         <v>-126751.5397260274</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="Q12" s="5">
         <v>1870.2465753424658</v>
       </c>
-      <c r="R12" s="4">
+      <c r="R12" s="5">
         <v>125024.44931506849</v>
       </c>
-      <c r="S12" s="4">
+      <c r="S12" s="5">
         <v>17495.635616438354</v>
       </c>
-      <c r="T12" s="4">
+      <c r="T12" s="5">
         <v>38348.342465753427</v>
       </c>
-      <c r="U12" s="4">
-        <v>0</v>
-      </c>
-      <c r="V12" s="4">
+      <c r="U12" s="5">
+        <v>0</v>
+      </c>
+      <c r="V12" s="5">
         <v>179.46301369863014</v>
       </c>
-      <c r="W12" s="4">
+      <c r="W12" s="5">
         <v>4472.3780821917808</v>
       </c>
-      <c r="X12" s="4">
+      <c r="X12" s="5">
         <v>187390.51506849314</v>
       </c>
-      <c r="Y12" s="4">
+      <c r="Y12" s="5">
         <v>41019.57808219178</v>
       </c>
-      <c r="Z12" s="4">
+      <c r="Z12" s="5">
         <v>32084.997260273973</v>
       </c>
-      <c r="AA12" s="4">
+      <c r="AA12" s="5">
         <v>23985.868493150687</v>
       </c>
-      <c r="AB12" s="4">
+      <c r="AB12" s="5">
         <v>6338.4383561643835</v>
       </c>
-      <c r="AC12" s="4">
+      <c r="AC12" s="5">
         <v>4103.5753424657532</v>
       </c>
-      <c r="AD12" s="4">
+      <c r="AD12" s="5">
         <v>3860.345205479452</v>
       </c>
-      <c r="AE12" s="4">
+      <c r="AE12" s="5">
         <v>66455.94794520548</v>
       </c>
-      <c r="AF12" s="4">
+      <c r="AF12" s="5">
         <v>177848.75068493153</v>
       </c>
-      <c r="AG12" s="4">
+      <c r="AG12" s="5">
         <v>365239.26575342467</v>
       </c>
-      <c r="AH12" s="4">
+      <c r="AH12" s="5">
         <v>4022.495890410959</v>
       </c>
-      <c r="AI12" s="4">
+      <c r="AI12" s="5">
         <v>628661.9753424658</v>
       </c>
-      <c r="AJ12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK12" s="4">
+      <c r="AJ12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="5">
         <v>12848.427397260275</v>
       </c>
-      <c r="AL12" s="4">
+      <c r="AL12" s="5">
         <v>-480195.36986301374</v>
       </c>
-      <c r="AM12" s="4">
+      <c r="AM12" s="5">
         <v>165337.52876712329</v>
       </c>
-      <c r="AN12" s="4">
+      <c r="AN12" s="5">
         <v>8607.038356164383</v>
       </c>
-      <c r="AO12" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP12" s="4">
+      <c r="AO12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP12" s="5">
         <v>27663.534246575342</v>
       </c>
-      <c r="AQ12" s="4">
+      <c r="AQ12" s="5">
         <v>9588.2000000000007</v>
       </c>
-      <c r="AR12" s="4">
+      <c r="AR12" s="5">
         <v>45858.772602739729</v>
       </c>
-      <c r="AS12" s="4">
+      <c r="AS12" s="5">
         <v>3875.6273972602739</v>
       </c>
-      <c r="AT12" s="4">
+      <c r="AT12" s="5">
         <v>11141.076712328768</v>
       </c>
-      <c r="AU12" s="4">
+      <c r="AU12" s="5">
         <v>29306.128767123286</v>
       </c>
-      <c r="AV12" s="4">
+      <c r="AV12" s="5">
         <v>55594.723287671237</v>
       </c>
-      <c r="AW12" s="4">
+      <c r="AW12" s="5">
         <v>2250.9178082191779</v>
       </c>
-      <c r="AX12" s="4">
+      <c r="AX12" s="5">
         <v>1296.4383561643835</v>
       </c>
-      <c r="AY12" s="4">
+      <c r="AY12" s="5">
         <v>26247.479452054795</v>
       </c>
-      <c r="AZ12" s="4">
+      <c r="AZ12" s="5">
         <v>17403.876712328769</v>
       </c>
-      <c r="BA12" s="4">
+      <c r="BA12" s="5">
         <v>6926.6958904109588</v>
       </c>
-      <c r="BB12" s="4">
+      <c r="BB12" s="5">
         <v>154042.96438356166</v>
       </c>
-      <c r="BC12" s="4">
+      <c r="BC12" s="5">
         <v>199901.73698630137</v>
       </c>
-      <c r="BD12" s="4">
+      <c r="BD12" s="5">
         <v>365239.26575342467</v>
       </c>
     </row>
     <row r="13" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="6">
         <v>44834</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="5">
         <v>202216.78630136987</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="5">
         <v>-228096.27945205479</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="5">
         <v>-25879.493150684932</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="5">
         <v>-53621.876712328769</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="5">
         <v>-60878.731506849312</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="5">
         <v>-40726.731506849319</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="5">
         <v>145.61917808219178</v>
       </c>
-      <c r="I13" s="4">
-        <v>0</v>
-      </c>
-      <c r="J13" s="4">
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
         <v>-180961.21369863013</v>
       </c>
-      <c r="K13" s="4">
-        <v>0</v>
-      </c>
-      <c r="L13" s="4">
+      <c r="K13" s="5">
+        <v>0</v>
+      </c>
+      <c r="L13" s="5">
         <v>1839.7589041095889</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13" s="5">
         <v>-2965.9945205479453</v>
       </c>
-      <c r="N13" s="4">
+      <c r="N13" s="5">
         <v>-182087.44931506849</v>
       </c>
-      <c r="O13" s="4">
+      <c r="O13" s="5">
         <v>4799.6794520547946</v>
       </c>
-      <c r="P13" s="4">
+      <c r="P13" s="5">
         <v>-177287.7698630137</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="Q13" s="5">
         <v>935.1232876712329</v>
       </c>
-      <c r="R13" s="4">
+      <c r="R13" s="5">
         <v>123678.22465753424</v>
       </c>
-      <c r="S13" s="4">
+      <c r="S13" s="5">
         <v>18131.317808219177</v>
       </c>
-      <c r="T13" s="4">
+      <c r="T13" s="5">
         <v>40964.671232876717</v>
       </c>
-      <c r="U13" s="4">
-        <v>0</v>
-      </c>
-      <c r="V13" s="4">
+      <c r="U13" s="5">
+        <v>0</v>
+      </c>
+      <c r="V13" s="5">
         <v>89.731506849315068</v>
       </c>
-      <c r="W13" s="4">
+      <c r="W13" s="5">
         <v>4633.1890410958904</v>
       </c>
-      <c r="X13" s="4">
+      <c r="X13" s="5">
         <v>188432.25753424657</v>
       </c>
-      <c r="Y13" s="4">
+      <c r="Y13" s="5">
         <v>43590.789041095893</v>
       </c>
-      <c r="Z13" s="4">
+      <c r="Z13" s="5">
         <v>30674.498630136986</v>
       </c>
-      <c r="AA13" s="4">
+      <c r="AA13" s="5">
         <v>21969.934246575343</v>
       </c>
-      <c r="AB13" s="4">
+      <c r="AB13" s="5">
         <v>6618.2191780821922</v>
       </c>
-      <c r="AC13" s="4">
+      <c r="AC13" s="5">
         <v>4068.2876712328766</v>
       </c>
-      <c r="AD13" s="4">
+      <c r="AD13" s="5">
         <v>4575.1726027397262</v>
       </c>
-      <c r="AE13" s="4">
+      <c r="AE13" s="5">
         <v>49776.47397260274</v>
       </c>
-      <c r="AF13" s="4">
+      <c r="AF13" s="5">
         <v>161273.37534246576</v>
       </c>
-      <c r="AG13" s="4">
+      <c r="AG13" s="5">
         <v>349705.63287671236</v>
       </c>
-      <c r="AH13" s="4">
+      <c r="AH13" s="5">
         <v>4206.7479452054795</v>
       </c>
-      <c r="AI13" s="4">
+      <c r="AI13" s="5">
         <v>652583.4876712329</v>
       </c>
-      <c r="AJ13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK13" s="4">
+      <c r="AJ13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="5">
         <v>15674.213698630138</v>
       </c>
-      <c r="AL13" s="4">
+      <c r="AL13" s="5">
         <v>-537396.68493150687</v>
       </c>
-      <c r="AM13" s="4">
+      <c r="AM13" s="5">
         <v>135067.76438356165</v>
       </c>
-      <c r="AN13" s="4">
+      <c r="AN13" s="5">
         <v>7746.0191780821915</v>
       </c>
-      <c r="AO13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP13" s="4">
+      <c r="AO13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP13" s="5">
         <v>30022.767123287671</v>
       </c>
-      <c r="AQ13" s="4">
+      <c r="AQ13" s="5">
         <v>9054.6</v>
       </c>
-      <c r="AR13" s="4">
+      <c r="AR13" s="5">
         <v>46823.386301369865</v>
       </c>
-      <c r="AS13" s="4">
+      <c r="AS13" s="5">
         <v>4051.813698630137</v>
       </c>
-      <c r="AT13" s="4">
+      <c r="AT13" s="5">
         <v>11811.038356164383</v>
       </c>
-      <c r="AU13" s="4">
+      <c r="AU13" s="5">
         <v>28531.564383561643</v>
       </c>
-      <c r="AV13" s="4">
+      <c r="AV13" s="5">
         <v>53526.361643835618</v>
       </c>
-      <c r="AW13" s="4">
+      <c r="AW13" s="5">
         <v>2255.9589041095887</v>
       </c>
-      <c r="AX13" s="4">
+      <c r="AX13" s="5">
         <v>1208.2191780821918</v>
       </c>
-      <c r="AY13" s="4">
+      <c r="AY13" s="5">
         <v>39588.739726027401</v>
       </c>
-      <c r="AZ13" s="4">
+      <c r="AZ13" s="5">
         <v>16675.438356164384</v>
       </c>
-      <c r="BA13" s="4">
+      <c r="BA13" s="5">
         <v>10165.34794520548</v>
       </c>
-      <c r="BB13" s="4">
+      <c r="BB13" s="5">
         <v>167814.48219178081</v>
       </c>
-      <c r="BC13" s="4">
+      <c r="BC13" s="5">
         <v>214637.86849315069</v>
       </c>
-      <c r="BD13" s="4">
+      <c r="BD13" s="5">
         <v>349705.63287671236</v>
       </c>
     </row>
     <row r="14" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="6">
         <v>44926</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="5">
         <v>198379</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="5">
         <v>-249498</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="5">
         <v>-51119</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="5">
         <v>-63297</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="5">
         <v>-73945</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="5">
         <v>-43765</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="5">
         <v>131</v>
       </c>
-      <c r="I14" s="4">
-        <v>0</v>
-      </c>
-      <c r="J14" s="4">
+      <c r="I14" s="5">
+        <v>0</v>
+      </c>
+      <c r="J14" s="5">
         <v>-231995</v>
       </c>
-      <c r="K14" s="4">
-        <v>0</v>
-      </c>
-      <c r="L14" s="4">
+      <c r="K14" s="5">
+        <v>0</v>
+      </c>
+      <c r="L14" s="5">
         <v>1900</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14" s="5">
         <v>-2844</v>
       </c>
-      <c r="N14" s="4">
+      <c r="N14" s="5">
         <v>-232939</v>
       </c>
-      <c r="O14" s="4">
+      <c r="O14" s="5">
         <v>5115</v>
       </c>
-      <c r="P14" s="4">
+      <c r="P14" s="5">
         <v>-227824</v>
       </c>
-      <c r="Q14" s="4">
-        <v>0</v>
-      </c>
-      <c r="R14" s="4">
+      <c r="Q14" s="5">
+        <v>0</v>
+      </c>
+      <c r="R14" s="5">
         <v>122332</v>
       </c>
-      <c r="S14" s="4">
+      <c r="S14" s="5">
         <v>18767</v>
       </c>
-      <c r="T14" s="4">
+      <c r="T14" s="5">
         <v>43581</v>
       </c>
-      <c r="U14" s="4">
-        <v>0</v>
-      </c>
-      <c r="V14" s="4">
-        <v>0</v>
-      </c>
-      <c r="W14" s="4">
+      <c r="U14" s="5">
+        <v>0</v>
+      </c>
+      <c r="V14" s="5">
+        <v>0</v>
+      </c>
+      <c r="W14" s="5">
         <v>4794</v>
       </c>
-      <c r="X14" s="4">
+      <c r="X14" s="5">
         <v>189474</v>
       </c>
-      <c r="Y14" s="4">
+      <c r="Y14" s="5">
         <v>46162</v>
       </c>
-      <c r="Z14" s="4">
+      <c r="Z14" s="5">
         <v>29264</v>
       </c>
-      <c r="AA14" s="4">
+      <c r="AA14" s="5">
         <v>19954</v>
       </c>
-      <c r="AB14" s="4">
+      <c r="AB14" s="5">
         <v>6898</v>
       </c>
-      <c r="AC14" s="4">
+      <c r="AC14" s="5">
         <v>4033</v>
       </c>
-      <c r="AD14" s="4">
+      <c r="AD14" s="5">
         <v>5290</v>
       </c>
-      <c r="AE14" s="4">
+      <c r="AE14" s="5">
         <v>33097</v>
       </c>
-      <c r="AF14" s="4">
+      <c r="AF14" s="5">
         <v>144698</v>
       </c>
-      <c r="AG14" s="4">
+      <c r="AG14" s="5">
         <v>334172</v>
       </c>
-      <c r="AH14" s="4">
+      <c r="AH14" s="5">
         <v>4391</v>
       </c>
-      <c r="AI14" s="4">
+      <c r="AI14" s="5">
         <v>676505</v>
       </c>
-      <c r="AJ14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK14" s="4">
+      <c r="AJ14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="5">
         <v>18500</v>
       </c>
-      <c r="AL14" s="4">
+      <c r="AL14" s="5">
         <v>-594598</v>
       </c>
-      <c r="AM14" s="4">
+      <c r="AM14" s="5">
         <v>104798</v>
       </c>
-      <c r="AN14" s="4">
+      <c r="AN14" s="5">
         <v>6885</v>
       </c>
-      <c r="AO14" s="4">
-        <v>0</v>
-      </c>
-      <c r="AP14" s="4">
+      <c r="AO14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP14" s="5">
         <v>32382</v>
       </c>
-      <c r="AQ14" s="4">
+      <c r="AQ14" s="5">
         <v>8521</v>
       </c>
-      <c r="AR14" s="4">
+      <c r="AR14" s="5">
         <v>47788</v>
       </c>
-      <c r="AS14" s="4">
+      <c r="AS14" s="5">
         <v>4228</v>
       </c>
-      <c r="AT14" s="4">
+      <c r="AT14" s="5">
         <v>12481</v>
       </c>
-      <c r="AU14" s="4">
+      <c r="AU14" s="5">
         <v>27757</v>
       </c>
-      <c r="AV14" s="4">
+      <c r="AV14" s="5">
         <v>51458</v>
       </c>
-      <c r="AW14" s="4">
+      <c r="AW14" s="5">
         <v>2261</v>
       </c>
-      <c r="AX14" s="4">
+      <c r="AX14" s="5">
         <v>1120</v>
       </c>
-      <c r="AY14" s="4">
+      <c r="AY14" s="5">
         <v>52930</v>
       </c>
-      <c r="AZ14" s="4">
+      <c r="AZ14" s="5">
         <v>15947</v>
       </c>
-      <c r="BA14" s="4">
+      <c r="BA14" s="5">
         <v>13404</v>
       </c>
-      <c r="BB14" s="4">
+      <c r="BB14" s="5">
         <v>181586</v>
       </c>
-      <c r="BC14" s="4">
+      <c r="BC14" s="5">
         <v>229374</v>
       </c>
-      <c r="BD14" s="4">
+      <c r="BD14" s="5">
         <v>334172</v>
       </c>
     </row>
     <row r="15" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="6">
         <v>45016</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="5">
         <v>208109.35616438356</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="5">
         <v>-242033.42465753423</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="5">
         <v>-33924.068493150684</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="5">
         <v>-53746.150684931505</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="5">
         <v>-65551.57534246576</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="5">
         <v>-47427.136986301368</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="5">
         <v>5043.2739726027403</v>
       </c>
-      <c r="I15" s="4">
-        <v>0</v>
-      </c>
-      <c r="J15" s="4">
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
         <v>-195605.65753424657</v>
       </c>
-      <c r="K15" s="4">
-        <v>0</v>
-      </c>
-      <c r="L15" s="4">
+      <c r="K15" s="5">
+        <v>0</v>
+      </c>
+      <c r="L15" s="5">
         <v>5558.1917808219168</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15" s="5">
         <v>-8663.6712328767135</v>
       </c>
-      <c r="N15" s="4">
+      <c r="N15" s="5">
         <v>-198711.13698630137</v>
       </c>
-      <c r="O15" s="4">
+      <c r="O15" s="5">
         <v>4229.7945205479455</v>
       </c>
-      <c r="P15" s="4">
+      <c r="P15" s="5">
         <v>-194481.34246575343</v>
       </c>
-      <c r="Q15" s="4">
-        <v>0</v>
-      </c>
-      <c r="R15" s="4">
+      <c r="Q15" s="5">
+        <v>0</v>
+      </c>
+      <c r="R15" s="5">
         <v>114962.10958904109</v>
       </c>
-      <c r="S15" s="4">
+      <c r="S15" s="5">
         <v>16890.31506849315</v>
       </c>
-      <c r="T15" s="4">
+      <c r="T15" s="5">
         <v>40231.767123287675</v>
       </c>
-      <c r="U15" s="4">
-        <v>0</v>
-      </c>
-      <c r="V15" s="4">
-        <v>0</v>
-      </c>
-      <c r="W15" s="4">
+      <c r="U15" s="5">
+        <v>0</v>
+      </c>
+      <c r="V15" s="5">
+        <v>0</v>
+      </c>
+      <c r="W15" s="5">
         <v>4795.4794520547948</v>
       </c>
-      <c r="X15" s="4">
+      <c r="X15" s="5">
         <v>176879.67123287672</v>
       </c>
-      <c r="Y15" s="4">
+      <c r="Y15" s="5">
         <v>45499.452054794521</v>
       </c>
-      <c r="Z15" s="4">
+      <c r="Z15" s="5">
         <v>27612.68493150685</v>
       </c>
-      <c r="AA15" s="4">
+      <c r="AA15" s="5">
         <v>21283.287671232876</v>
       </c>
-      <c r="AB15" s="4">
+      <c r="AB15" s="5">
         <v>5688.301369863013</v>
       </c>
-      <c r="AC15" s="4">
+      <c r="AC15" s="5">
         <v>4203.6301369863013</v>
       </c>
-      <c r="AD15" s="4">
+      <c r="AD15" s="5">
         <v>5127.5068493150684</v>
       </c>
-      <c r="AE15" s="4">
+      <c r="AE15" s="5">
         <v>39996.178082191778</v>
       </c>
-      <c r="AF15" s="4">
+      <c r="AF15" s="5">
         <v>149411.0410958904</v>
       </c>
-      <c r="AG15" s="4">
+      <c r="AG15" s="5">
         <v>326290.71232876711</v>
       </c>
-      <c r="AH15" s="4">
+      <c r="AH15" s="5">
         <v>5736.3150684931506</v>
       </c>
-      <c r="AI15" s="4">
+      <c r="AI15" s="5">
         <v>699337.1369863014</v>
       </c>
-      <c r="AJ15" s="4">
+      <c r="AJ15" s="5">
         <v>28.109589041095894</v>
       </c>
-      <c r="AK15" s="4">
+      <c r="AK15" s="5">
         <v>18357.232876712329</v>
       </c>
-      <c r="AL15" s="4">
+      <c r="AL15" s="5">
         <v>-617431.12328767125</v>
       </c>
-      <c r="AM15" s="4">
+      <c r="AM15" s="5">
         <v>106027.67123287672</v>
       </c>
-      <c r="AN15" s="4">
+      <c r="AN15" s="5">
         <v>18275.054794520547</v>
       </c>
-      <c r="AO15" s="4">
+      <c r="AO15" s="5">
         <v>1.7706575342465751</v>
       </c>
-      <c r="AP15" s="4">
+      <c r="AP15" s="5">
         <v>29620.35616438356</v>
       </c>
-      <c r="AQ15" s="4">
+      <c r="AQ15" s="5">
         <v>8475.6301369863013</v>
       </c>
-      <c r="AR15" s="4">
+      <c r="AR15" s="5">
         <v>58141.698630136983</v>
       </c>
-      <c r="AS15" s="4">
+      <c r="AS15" s="5">
         <v>4264.2465753424658</v>
       </c>
-      <c r="AT15" s="4">
+      <c r="AT15" s="5">
         <v>12347.602739726028</v>
       </c>
-      <c r="AU15" s="4">
+      <c r="AU15" s="5">
         <v>25291.246575342466</v>
       </c>
-      <c r="AV15" s="4">
+      <c r="AV15" s="5">
         <v>50895.808219178085</v>
       </c>
-      <c r="AW15" s="4">
+      <c r="AW15" s="5">
         <v>2131.7945205479455</v>
       </c>
-      <c r="AX15" s="4">
+      <c r="AX15" s="5">
         <v>1100.7671232876712</v>
       </c>
-      <c r="AY15" s="4">
+      <c r="AY15" s="5">
         <v>39917.232876712325</v>
       </c>
-      <c r="AZ15" s="4">
+      <c r="AZ15" s="5">
         <v>14880.068493150684</v>
       </c>
-      <c r="BA15" s="4">
+      <c r="BA15" s="5">
         <v>11292.575342465754</v>
       </c>
-      <c r="BB15" s="4">
+      <c r="BB15" s="5">
         <v>162121.34246575343</v>
       </c>
-      <c r="BC15" s="4">
+      <c r="BC15" s="5">
         <v>220263.0410958904</v>
       </c>
-      <c r="BD15" s="4">
+      <c r="BD15" s="5">
         <v>326290.71232876711</v>
       </c>
     </row>
     <row r="16" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="6">
         <v>45107</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="5">
         <v>217947.82739726026</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="5">
         <v>-234485.90958904108</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="5">
         <v>-16538.082191780821</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="5">
         <v>-44089.180821917806</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="5">
         <v>-57064.890410958906</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="5">
         <v>-51129.964383561644</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="5">
         <v>10010.128767123288</v>
       </c>
-      <c r="I16" s="4">
-        <v>0</v>
-      </c>
-      <c r="J16" s="4">
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
         <v>-158811.98904109589</v>
       </c>
-      <c r="K16" s="4">
-        <v>0</v>
-      </c>
-      <c r="L16" s="4">
+      <c r="K16" s="5">
+        <v>0</v>
+      </c>
+      <c r="L16" s="5">
         <v>9257.0301369863009</v>
       </c>
-      <c r="M16" s="4">
+      <c r="M16" s="5">
         <v>-14548.005479452055</v>
       </c>
-      <c r="N16" s="4">
+      <c r="N16" s="5">
         <v>-164102.96438356163</v>
       </c>
-      <c r="O16" s="4">
+      <c r="O16" s="5">
         <v>3334.7534246575342</v>
       </c>
-      <c r="P16" s="4">
+      <c r="P16" s="5">
         <v>-160768.21095890412</v>
       </c>
-      <c r="Q16" s="4">
-        <v>0</v>
-      </c>
-      <c r="R16" s="4">
+      <c r="Q16" s="5">
+        <v>0</v>
+      </c>
+      <c r="R16" s="5">
         <v>107510.33150684931</v>
       </c>
-      <c r="S16" s="4">
+      <c r="S16" s="5">
         <v>14992.77808219178</v>
       </c>
-      <c r="T16" s="4">
+      <c r="T16" s="5">
         <v>36845.320547945208</v>
       </c>
-      <c r="U16" s="4">
-        <v>0</v>
-      </c>
-      <c r="V16" s="4">
-        <v>0</v>
-      </c>
-      <c r="W16" s="4">
+      <c r="U16" s="5">
+        <v>0</v>
+      </c>
+      <c r="V16" s="5">
+        <v>0</v>
+      </c>
+      <c r="W16" s="5">
         <v>4796.9753424657538</v>
       </c>
-      <c r="X16" s="4">
+      <c r="X16" s="5">
         <v>164145.40547945205</v>
       </c>
-      <c r="Y16" s="4">
+      <c r="Y16" s="5">
         <v>44829.542465753424</v>
       </c>
-      <c r="Z16" s="4">
+      <c r="Z16" s="5">
         <v>25943.021917808219</v>
       </c>
-      <c r="AA16" s="4">
+      <c r="AA16" s="5">
         <v>22627.345205479451</v>
       </c>
-      <c r="AB16" s="4">
+      <c r="AB16" s="5">
         <v>4465.1616438356159</v>
       </c>
-      <c r="AC16" s="4">
+      <c r="AC16" s="5">
         <v>4376.1561643835612</v>
       </c>
-      <c r="AD16" s="4">
+      <c r="AD16" s="5">
         <v>4963.2082191780819</v>
       </c>
-      <c r="AE16" s="4">
+      <c r="AE16" s="5">
         <v>46972.013698630137</v>
       </c>
-      <c r="AF16" s="4">
+      <c r="AF16" s="5">
         <v>154176.44931506849</v>
       </c>
-      <c r="AG16" s="4">
+      <c r="AG16" s="5">
         <v>318321.85479452054</v>
       </c>
-      <c r="AH16" s="4">
+      <c r="AH16" s="5">
         <v>7096.5780821917806</v>
       </c>
-      <c r="AI16" s="4">
+      <c r="AI16" s="5">
         <v>722422.96438356163</v>
       </c>
-      <c r="AJ16" s="4">
+      <c r="AJ16" s="5">
         <v>56.531506849315072</v>
       </c>
-      <c r="AK16" s="4">
+      <c r="AK16" s="5">
         <v>18212.879452054796</v>
       </c>
-      <c r="AL16" s="4">
+      <c r="AL16" s="5">
         <v>-640517.94794520549</v>
       </c>
-      <c r="AM16" s="4">
+      <c r="AM16" s="5">
         <v>107271.00547945205</v>
       </c>
-      <c r="AN16" s="4">
+      <c r="AN16" s="5">
         <v>29791.665753424655</v>
       </c>
-      <c r="AO16" s="4">
+      <c r="AO16" s="5">
         <v>3.56098904109589</v>
       </c>
-      <c r="AP16" s="4">
+      <c r="AP16" s="5">
         <v>26828.027397260274</v>
       </c>
-      <c r="AQ16" s="4">
+      <c r="AQ16" s="5">
         <v>8429.7561643835616</v>
       </c>
-      <c r="AR16" s="4">
+      <c r="AR16" s="5">
         <v>68610.438356164377</v>
       </c>
-      <c r="AS16" s="4">
+      <c r="AS16" s="5">
         <v>4300.8958904109586</v>
       </c>
-      <c r="AT16" s="4">
+      <c r="AT16" s="5">
         <v>12212.723287671233</v>
       </c>
-      <c r="AU16" s="4">
+      <c r="AU16" s="5">
         <v>22798.095890410958</v>
       </c>
-      <c r="AV16" s="4">
+      <c r="AV16" s="5">
         <v>50327.369863013701</v>
       </c>
-      <c r="AW16" s="4">
+      <c r="AW16" s="5">
         <v>2001.1534246575343</v>
       </c>
-      <c r="AX16" s="4">
+      <c r="AX16" s="5">
         <v>1081.3205479452056</v>
       </c>
-      <c r="AY16" s="4">
+      <c r="AY16" s="5">
         <v>26759.879452054793</v>
       </c>
-      <c r="AZ16" s="4">
+      <c r="AZ16" s="5">
         <v>13801.282191780821</v>
       </c>
-      <c r="BA16" s="4">
+      <c r="BA16" s="5">
         <v>9157.690410958905</v>
       </c>
-      <c r="BB16" s="4">
+      <c r="BB16" s="5">
         <v>142440.4109589041</v>
       </c>
-      <c r="BC16" s="4">
+      <c r="BC16" s="5">
         <v>211050.84931506848</v>
       </c>
-      <c r="BD16" s="4">
+      <c r="BD16" s="5">
         <v>318321.85479452054</v>
       </c>
     </row>
     <row r="17" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="6">
         <v>45199</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="5">
         <v>227894.41369863012</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="5">
         <v>-226855.45479452054</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="5">
         <v>1038.9589041095896</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="5">
         <v>-34326.090410958903</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="5">
         <v>-48484.945205479453</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="5">
         <v>-54873.482191780822</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="5">
         <v>15031.564383561643</v>
       </c>
-      <c r="I17" s="4">
-        <v>0</v>
-      </c>
-      <c r="J17" s="4">
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
         <v>-121613.99452054795</v>
       </c>
-      <c r="K17" s="4">
-        <v>0</v>
-      </c>
-      <c r="L17" s="4">
+      <c r="K17" s="5">
+        <v>0</v>
+      </c>
+      <c r="L17" s="5">
         <v>12996.51506849315</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17" s="5">
         <v>-20497.002739726027</v>
       </c>
-      <c r="N17" s="4">
+      <c r="N17" s="5">
         <v>-129114.48219178081</v>
       </c>
-      <c r="O17" s="4">
+      <c r="O17" s="5">
         <v>2429.8767123287671</v>
       </c>
-      <c r="P17" s="4">
+      <c r="P17" s="5">
         <v>-126684.60547945206</v>
       </c>
-      <c r="Q17" s="4">
-        <v>0</v>
-      </c>
-      <c r="R17" s="4">
+      <c r="Q17" s="5">
+        <v>0</v>
+      </c>
+      <c r="R17" s="5">
         <v>99976.665753424662</v>
       </c>
-      <c r="S17" s="4">
+      <c r="S17" s="5">
         <v>13074.38904109589</v>
       </c>
-      <c r="T17" s="4">
+      <c r="T17" s="5">
         <v>33421.660273972608</v>
       </c>
-      <c r="U17" s="4">
-        <v>0</v>
-      </c>
-      <c r="V17" s="4">
-        <v>0</v>
-      </c>
-      <c r="W17" s="4">
+      <c r="U17" s="5">
+        <v>0</v>
+      </c>
+      <c r="V17" s="5">
+        <v>0</v>
+      </c>
+      <c r="W17" s="5">
         <v>4798.4876712328769</v>
       </c>
-      <c r="X17" s="4">
+      <c r="X17" s="5">
         <v>151271.20273972602</v>
       </c>
-      <c r="Y17" s="4">
+      <c r="Y17" s="5">
         <v>44152.271232876708</v>
       </c>
-      <c r="Z17" s="4">
+      <c r="Z17" s="5">
         <v>24255.010958904109</v>
       </c>
-      <c r="AA17" s="4">
+      <c r="AA17" s="5">
         <v>23986.172602739724</v>
       </c>
-      <c r="AB17" s="4">
+      <c r="AB17" s="5">
         <v>3228.580821917808</v>
       </c>
-      <c r="AC17" s="4">
+      <c r="AC17" s="5">
         <v>4550.5780821917806</v>
       </c>
-      <c r="AD17" s="4">
+      <c r="AD17" s="5">
         <v>4797.1041095890414</v>
       </c>
-      <c r="AE17" s="4">
+      <c r="AE17" s="5">
         <v>54024.506849315068</v>
       </c>
-      <c r="AF17" s="4">
+      <c r="AF17" s="5">
         <v>158994.22465753424</v>
       </c>
-      <c r="AG17" s="4">
+      <c r="AG17" s="5">
         <v>310265.42739726027</v>
       </c>
-      <c r="AH17" s="4">
+      <c r="AH17" s="5">
         <v>8471.7890410958898</v>
       </c>
-      <c r="AI17" s="4">
+      <c r="AI17" s="5">
         <v>745762.48219178081</v>
       </c>
-      <c r="AJ17" s="4">
+      <c r="AJ17" s="5">
         <v>85.265753424657532</v>
       </c>
-      <c r="AK17" s="4">
+      <c r="AK17" s="5">
         <v>18066.939726027398</v>
       </c>
-      <c r="AL17" s="4">
+      <c r="AL17" s="5">
         <v>-663858.47397260275</v>
       </c>
-      <c r="AM17" s="4">
+      <c r="AM17" s="5">
         <v>108528.00273972603</v>
       </c>
-      <c r="AN17" s="4">
+      <c r="AN17" s="5">
         <v>41434.832876712331</v>
       </c>
-      <c r="AO17" s="4">
+      <c r="AO17" s="5">
         <v>5.3709945205479448</v>
       </c>
-      <c r="AP17" s="4">
+      <c r="AP17" s="5">
         <v>24005.013698630137</v>
       </c>
-      <c r="AQ17" s="4">
+      <c r="AQ17" s="5">
         <v>8383.3780821917808</v>
       </c>
-      <c r="AR17" s="4">
+      <c r="AR17" s="5">
         <v>79194.219178082189</v>
       </c>
-      <c r="AS17" s="4">
+      <c r="AS17" s="5">
         <v>4337.9479452054793</v>
       </c>
-      <c r="AT17" s="4">
+      <c r="AT17" s="5">
         <v>12076.361643835617</v>
       </c>
-      <c r="AU17" s="4">
+      <c r="AU17" s="5">
         <v>20277.547945205479</v>
       </c>
-      <c r="AV17" s="4">
+      <c r="AV17" s="5">
         <v>49752.684931506854</v>
       </c>
-      <c r="AW17" s="4">
+      <c r="AW17" s="5">
         <v>1869.0767123287671</v>
       </c>
-      <c r="AX17" s="4">
+      <c r="AX17" s="5">
         <v>1061.6602739726027</v>
       </c>
-      <c r="AY17" s="4">
+      <c r="AY17" s="5">
         <v>13457.939726027396</v>
       </c>
-      <c r="AZ17" s="4">
+      <c r="AZ17" s="5">
         <v>12710.641095890411</v>
       </c>
-      <c r="BA17" s="4">
+      <c r="BA17" s="5">
         <v>6999.3452054794525</v>
       </c>
-      <c r="BB17" s="4">
+      <c r="BB17" s="5">
         <v>122543.20547945205</v>
       </c>
-      <c r="BC17" s="4">
+      <c r="BC17" s="5">
         <v>201737.42465753423</v>
       </c>
-      <c r="BD17" s="4">
+      <c r="BD17" s="5">
         <v>310265.42739726027</v>
       </c>
     </row>
     <row r="18" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18" s="6">
         <v>45291</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="5">
         <v>237841</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="5">
         <v>-219225</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="5">
         <v>18616</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="5">
         <v>-24563</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="5">
         <v>-39905</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="5">
         <v>-58617</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="5">
         <v>20053</v>
       </c>
-      <c r="I18" s="4">
-        <v>0</v>
-      </c>
-      <c r="J18" s="4">
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
         <v>-84416</v>
       </c>
-      <c r="K18" s="4">
-        <v>0</v>
-      </c>
-      <c r="L18" s="4">
+      <c r="K18" s="5">
+        <v>0</v>
+      </c>
+      <c r="L18" s="5">
         <v>16736</v>
       </c>
-      <c r="M18" s="4">
+      <c r="M18" s="5">
         <v>-26446</v>
       </c>
-      <c r="N18" s="4">
+      <c r="N18" s="5">
         <v>-94126</v>
       </c>
-      <c r="O18" s="4">
+      <c r="O18" s="5">
         <v>1525</v>
       </c>
-      <c r="P18" s="4">
+      <c r="P18" s="5">
         <v>-92601</v>
       </c>
-      <c r="Q18" s="4">
-        <v>0</v>
-      </c>
-      <c r="R18" s="4">
+      <c r="Q18" s="5">
+        <v>0</v>
+      </c>
+      <c r="R18" s="5">
         <v>92443</v>
       </c>
-      <c r="S18" s="4">
+      <c r="S18" s="5">
         <v>11156</v>
       </c>
-      <c r="T18" s="4">
+      <c r="T18" s="5">
         <v>29998</v>
       </c>
-      <c r="U18" s="4">
-        <v>0</v>
-      </c>
-      <c r="V18" s="4">
-        <v>0</v>
-      </c>
-      <c r="W18" s="4">
+      <c r="U18" s="5">
+        <v>0</v>
+      </c>
+      <c r="V18" s="5">
+        <v>0</v>
+      </c>
+      <c r="W18" s="5">
         <v>4800</v>
       </c>
-      <c r="X18" s="4">
+      <c r="X18" s="5">
         <v>138397</v>
       </c>
-      <c r="Y18" s="4">
+      <c r="Y18" s="5">
         <v>43475</v>
       </c>
-      <c r="Z18" s="4">
+      <c r="Z18" s="5">
         <v>22567</v>
       </c>
-      <c r="AA18" s="4">
+      <c r="AA18" s="5">
         <v>25345</v>
       </c>
-      <c r="AB18" s="4">
+      <c r="AB18" s="5">
         <v>1992</v>
       </c>
-      <c r="AC18" s="4">
+      <c r="AC18" s="5">
         <v>4725</v>
       </c>
-      <c r="AD18" s="4">
+      <c r="AD18" s="5">
         <v>4631</v>
       </c>
-      <c r="AE18" s="4">
+      <c r="AE18" s="5">
         <v>61077</v>
       </c>
-      <c r="AF18" s="4">
+      <c r="AF18" s="5">
         <v>163812</v>
       </c>
-      <c r="AG18" s="4">
+      <c r="AG18" s="5">
         <v>302209</v>
       </c>
-      <c r="AH18" s="4">
+      <c r="AH18" s="5">
         <v>9847</v>
       </c>
-      <c r="AI18" s="4">
+      <c r="AI18" s="5">
         <v>769102</v>
       </c>
-      <c r="AJ18" s="4">
+      <c r="AJ18" s="5">
         <v>114</v>
       </c>
-      <c r="AK18" s="4">
+      <c r="AK18" s="5">
         <v>17921</v>
       </c>
-      <c r="AL18" s="4">
+      <c r="AL18" s="5">
         <v>-687199</v>
       </c>
-      <c r="AM18" s="4">
+      <c r="AM18" s="5">
         <v>109785</v>
       </c>
-      <c r="AN18" s="4">
+      <c r="AN18" s="5">
         <v>53078</v>
       </c>
-      <c r="AO18" s="4">
+      <c r="AO18" s="5">
         <v>7.181</v>
       </c>
-      <c r="AP18" s="4">
+      <c r="AP18" s="5">
         <v>21182</v>
       </c>
-      <c r="AQ18" s="4">
+      <c r="AQ18" s="5">
         <v>8337</v>
       </c>
-      <c r="AR18" s="4">
+      <c r="AR18" s="5">
         <v>89778</v>
       </c>
-      <c r="AS18" s="4">
+      <c r="AS18" s="5">
         <v>4375</v>
       </c>
-      <c r="AT18" s="4">
+      <c r="AT18" s="5">
         <v>11940</v>
       </c>
-      <c r="AU18" s="4">
+      <c r="AU18" s="5">
         <v>17757</v>
       </c>
-      <c r="AV18" s="4">
+      <c r="AV18" s="5">
         <v>49178</v>
       </c>
-      <c r="AW18" s="4">
+      <c r="AW18" s="5">
         <v>1737</v>
       </c>
-      <c r="AX18" s="4">
+      <c r="AX18" s="5">
         <v>1042</v>
       </c>
-      <c r="AY18" s="4">
+      <c r="AY18" s="5">
         <v>156</v>
       </c>
-      <c r="AZ18" s="4">
+      <c r="AZ18" s="5">
         <v>11620</v>
       </c>
-      <c r="BA18" s="4">
+      <c r="BA18" s="5">
         <v>4841</v>
       </c>
-      <c r="BB18" s="4">
+      <c r="BB18" s="5">
         <v>102646</v>
       </c>
-      <c r="BC18" s="4">
+      <c r="BC18" s="5">
         <v>192424</v>
       </c>
-      <c r="BD18" s="4">
+      <c r="BD18" s="5">
         <v>302209</v>
       </c>
     </row>
     <row r="19" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="22" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
+      <c r="B22" s="4"/>
     </row>
     <row r="24" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
+      <c r="B24" s="4"/>
     </row>
     <row r="26" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
+      <c r="B27" s="4"/>
     </row>
     <row r="29" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
+      <c r="B29" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
[UPDATE] GomSpace.xlsx change currency label for python interpretability
</commit_message>
<xml_diff>
--- a/financial_data/GomSpace.xlsx
+++ b/financial_data/GomSpace.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1085D7-6BE4-4DA1-8D2C-F412372116B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B980C7-AC3E-4438-BC44-1EC39729C81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D4168B6-43E9-4474-9A7A-6AA1A32D8675}"/>
   </bookViews>
@@ -202,8 +202,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="_([$SEK]\ * #,##0.00_);_([$SEK]\ * \(#,##0.00\);_([$SEK]\ * &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0.00\ [$kr-41D]_-;\-* #,##0.00\ [$kr-41D]_-;_-* &quot;-&quot;??\ [$kr-41D]_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -252,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -263,13 +263,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -606,7 +603,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885749C5-52DA-4D23-9415-6ADFFD56982C}">
-  <dimension ref="A1:BD29"/>
+  <dimension ref="A1:BD18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -822,7 +819,7 @@
       </c>
     </row>
     <row r="2" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="4">
         <v>43830</v>
       </c>
       <c r="B2" s="5">
@@ -992,7 +989,7 @@
       </c>
     </row>
     <row r="3" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+      <c r="A3" s="4">
         <v>43921</v>
       </c>
       <c r="B3" s="5">
@@ -1162,7 +1159,7 @@
       </c>
     </row>
     <row r="4" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+      <c r="A4" s="4">
         <v>44012</v>
       </c>
       <c r="B4" s="5">
@@ -1332,7 +1329,7 @@
       </c>
     </row>
     <row r="5" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>44104</v>
       </c>
       <c r="B5" s="5">
@@ -1502,7 +1499,7 @@
       </c>
     </row>
     <row r="6" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="A6" s="4">
         <v>44196</v>
       </c>
       <c r="B6" s="5">
@@ -1672,7 +1669,7 @@
       </c>
     </row>
     <row r="7" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+      <c r="A7" s="4">
         <v>44286</v>
       </c>
       <c r="B7" s="5">
@@ -1842,7 +1839,7 @@
       </c>
     </row>
     <row r="8" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+      <c r="A8" s="4">
         <v>44377</v>
       </c>
       <c r="B8" s="5">
@@ -2012,7 +2009,7 @@
       </c>
     </row>
     <row r="9" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+      <c r="A9" s="4">
         <v>44469</v>
       </c>
       <c r="B9" s="5">
@@ -2182,7 +2179,7 @@
       </c>
     </row>
     <row r="10" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="4">
         <v>44561</v>
       </c>
       <c r="B10" s="5">
@@ -2352,7 +2349,7 @@
       </c>
     </row>
     <row r="11" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="4">
         <v>44651</v>
       </c>
       <c r="B11" s="5">
@@ -2522,7 +2519,7 @@
       </c>
     </row>
     <row r="12" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="4">
         <v>44742</v>
       </c>
       <c r="B12" s="5">
@@ -2692,7 +2689,7 @@
       </c>
     </row>
     <row r="13" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="4">
         <v>44834</v>
       </c>
       <c r="B13" s="5">
@@ -2862,7 +2859,7 @@
       </c>
     </row>
     <row r="14" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="4">
         <v>44926</v>
       </c>
       <c r="B14" s="5">
@@ -3032,7 +3029,7 @@
       </c>
     </row>
     <row r="15" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="4">
         <v>45016</v>
       </c>
       <c r="B15" s="5">
@@ -3202,7 +3199,7 @@
       </c>
     </row>
     <row r="16" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="A16" s="4">
         <v>45107</v>
       </c>
       <c r="B16" s="5">
@@ -3372,7 +3369,7 @@
       </c>
     </row>
     <row r="17" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+      <c r="A17" s="4">
         <v>45199</v>
       </c>
       <c r="B17" s="5">
@@ -3542,7 +3539,7 @@
       </c>
     </row>
     <row r="18" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6">
+      <c r="A18" s="4">
         <v>45291</v>
       </c>
       <c r="B18" s="5">
@@ -3710,28 +3707,6 @@
       <c r="BD18" s="5">
         <v>302209</v>
       </c>
-    </row>
-    <row r="19" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="4"/>
-    </row>
-    <row r="22" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
-    </row>
-    <row r="24" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
-    </row>
-    <row r="26" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="4"/>
-    </row>
-    <row r="27" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
-    </row>
-    <row r="29" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
[UPDATE] GomSpace.xlsx headings to be consistent with other sheets
</commit_message>
<xml_diff>
--- a/financial_data/GomSpace.xlsx
+++ b/financial_data/GomSpace.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B980C7-AC3E-4438-BC44-1EC39729C81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B66BBB7-69B0-4F41-856C-3B0E48405390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D4168B6-43E9-4474-9A7A-6AA1A32D8675}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Quarter</t>
   </si>
   <si>
-    <t>Net revenue</t>
-  </si>
-  <si>
     <t>Cost of goods sold</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
     <t>Total current assets</t>
   </si>
   <si>
-    <t>Total assets</t>
-  </si>
-  <si>
     <t>Share capital</t>
   </si>
   <si>
@@ -152,9 +146,6 @@
     <t>Retained earnings</t>
   </si>
   <si>
-    <t>Total equity</t>
-  </si>
-  <si>
     <t>Credit institutions</t>
   </si>
   <si>
@@ -176,9 +167,6 @@
     <t>Total current liabilities</t>
   </si>
   <si>
-    <t>Total liabilities</t>
-  </si>
-  <si>
     <t>Total equity and liabilities</t>
   </si>
   <si>
@@ -195,6 +183,18 @@
   </si>
   <si>
     <t>Provision for contract work loss</t>
+  </si>
+  <si>
+    <t>Total Assets</t>
+  </si>
+  <si>
+    <t>Total Equity</t>
+  </si>
+  <si>
+    <t>Total Liabilities</t>
+  </si>
+  <si>
+    <t>Revenue</t>
   </si>
 </sst>
 </file>
@@ -605,7 +605,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885749C5-52DA-4D23-9415-6ADFFD56982C}">
   <dimension ref="A1:BD18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -653,169 +655,169 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="BA1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AK1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AR1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AS1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AU1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="BD1" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="BA1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="BB1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="BC1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="BD1" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[UPDATE] GomSpace.xlsx rn Profit (loss) for the year -> Net loss to be consistent with other data
</commit_message>
<xml_diff>
--- a/financial_data/GomSpace.xlsx
+++ b/financial_data/GomSpace.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B66BBB7-69B0-4F41-856C-3B0E48405390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3BC19A-E80F-445D-BEE1-09F4E3CE0B70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4D4168B6-43E9-4474-9A7A-6AA1A32D8675}"/>
   </bookViews>
@@ -82,10 +82,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Profit (loss) for the year</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Goodwill</t>
   </si>
   <si>
@@ -195,6 +191,9 @@
   </si>
   <si>
     <t>Revenue</t>
+  </si>
+  <si>
+    <t>Net loss</t>
   </si>
 </sst>
 </file>
@@ -605,9 +604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885749C5-52DA-4D23-9415-6ADFFD56982C}">
   <dimension ref="A1:BD18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -644,7 +641,8 @@
     <col min="42" max="44" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="46" max="48" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="51" max="53" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="54" max="56" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="57" max="16384" width="9" style="3"/>
@@ -655,7 +653,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -697,127 +695,127 @@
         <v>13</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AH1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AK1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AS1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="BB1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="BC1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AN1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="BA1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="BB1" s="2" t="s">
+      <c r="BD1" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="BC1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="BD1" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:56" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1133,7 +1131,7 @@
         <v>12743.592896174863</v>
       </c>
       <c r="AV3" s="5">
-        <v>32902.166666666672</v>
+        <v>32902.166666666701</v>
       </c>
       <c r="AW3" s="5">
         <v>3557.1584699453551</v>

</xml_diff>